<commit_message>
notes de cours 01/02/2024
</commit_message>
<xml_diff>
--- a/01022024.xlsx
+++ b/01022024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Formation\IFC Avignon\CSharp2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87D319A8-8F9A-47E6-810F-6A7839C85440}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E649BC5-C8FE-4BDB-9A1A-C1E376ABC2B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="90" windowWidth="28740" windowHeight="15510" xr2:uid="{2650DBA8-AD81-4DDE-9814-270D09113792}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="20">
   <si>
     <t>BEKTAS Zekarya</t>
   </si>
@@ -91,6 +91,9 @@
   </si>
   <si>
     <t>dotnet -v</t>
+  </si>
+  <si>
+    <t>run</t>
   </si>
 </sst>
 </file>
@@ -453,10 +456,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65294355-195D-45AC-B4EF-6C0017B43A3B}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -465,7 +468,7 @@
     <col min="3" max="3" width="33.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>14</v>
       </c>
@@ -481,8 +484,11 @@
       <c r="F1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -490,7 +496,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -501,7 +507,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -517,8 +523,14 @@
       <c r="E4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -537,8 +549,11 @@
       <c r="F5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -557,8 +572,11 @@
       <c r="F6" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -577,8 +595,11 @@
       <c r="F7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -595,6 +616,9 @@
         <v>3</v>
       </c>
       <c r="F8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G8" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>